<commit_message>
POM adding  <testFailureIgnore> and    <forkMode>none</forkMode> to work both in Windows and Ubuntu
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/TestData.xlsx
+++ b/src/test/resources/Excel Files/TestData.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21030"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C80242F-E7E1-4D3D-BC09-9DFE4567E9C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179020"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -31,29 +33,23 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Gladson</t>
-  </si>
-  <si>
-    <t>Antony</t>
-  </si>
-  <si>
     <t>TC_001</t>
   </si>
   <si>
+    <t>alistairzhu@gmail.com</t>
+  </si>
+  <si>
+    <t>1199myunipass9911</t>
+  </si>
+  <si>
     <t>TC_002</t>
-  </si>
-  <si>
-    <t>Gladson_Password</t>
-  </si>
-  <si>
-    <t>Antony_Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,29 +58,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -92,35 +82,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -149,7 +125,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -161,7 +137,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -208,6 +184,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -243,6 +236,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,68 +404,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9C2B1A9C-5DA9-490C-898F-34F5AD7A4757}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{8C5081F5-5596-4C59-96A0-BCA1BDEEB5F1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>